<commit_message>
Timeline for LID Board test fixture dev added
</commit_message>
<xml_diff>
--- a/Airzai TF Development.xlsx
+++ b/Airzai TF Development.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teamairzai-my.sharepoint.com/personal/kashif_airzai_com/Documents/Airzai/GitHub/Airzai-Hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajeeth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A033200-32CD-49B5-944C-85E35CA0FA07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D444314-A663-4925-8FAB-CD84D4FAC18C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>Objectives</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>TF Dev LED Strip, Sense Flex</t>
+  </si>
+  <si>
+    <t>TF Dev LID Board</t>
   </si>
 </sst>
 </file>
@@ -820,7 +823,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:XFD" xr:uid="{1CADD265-FFCF-4FA1-8675-14E97DE48D71}">
+  <autoFilter ref="A1" xr:uid="{1CADD265-FFCF-4FA1-8675-14E97DE48D71}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:XFD1048576">
       <sortCondition ref="C1:C1048576"/>
     </sortState>
@@ -835,7 +838,7 @@
   <dimension ref="C2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1034,7 @@
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
@@ -1045,10 +1048,10 @@
         <v>4</v>
       </c>
       <c r="F20" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="3">
-        <v>43614</v>
+        <v>43630</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
@@ -1059,10 +1062,10 @@
         <v>40</v>
       </c>
       <c r="F21" s="6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="3">
-        <v>43619</v>
+        <v>43633</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.25">
@@ -1073,10 +1076,10 @@
         <v>40</v>
       </c>
       <c r="F22" s="6">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="H22" s="3">
-        <v>43620</v>
+        <v>43634</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
@@ -1090,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="3">
-        <v>43621</v>
+        <v>43636</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
@@ -1101,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="7">
-        <v>43623</v>
+        <v>43637</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
@@ -1112,10 +1115,10 @@
         <v>40</v>
       </c>
       <c r="F25" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H25" s="7">
-        <v>43626</v>
+        <v>43641</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
@@ -1129,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="7">
-        <v>43627</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
@@ -1143,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="7">
-        <v>43627</v>
+        <v>43642</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
@@ -1157,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="7">
-        <v>43628</v>
+        <v>43644</v>
       </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.25">

</xml_diff>